<commit_message>
add CPLD with 64MCs
</commit_message>
<xml_diff>
--- a/pcb/BOM.xlsx
+++ b/pcb/BOM.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\Bartmann\Workspaces\Git\Eigenes\SNES-AddOn-PCBs\MultiRegion_with_DeJitter_QID\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Peter\Documents\Workspaces\GitHub\SNES_MultiRegion_with_DeJitter_QID\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB56C1D-260A-48E4-BC1D-19F3ACD32CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8850" yWindow="3120" windowWidth="23955" windowHeight="16320"/>
+    <workbookView xWindow="6315" yWindow="3915" windowWidth="25005" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMR20200325" sheetId="5" r:id="rId1"/>
     <sheet name="SMR20190813" sheetId="4" r:id="rId2"/>
     <sheet name="SMR20190603" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="191029" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -24,7 +25,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -35,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="155">
   <si>
     <t>Designator</t>
   </si>
@@ -485,12 +490,27 @@
   </si>
   <si>
     <t>SMR20200325</t>
+  </si>
+  <si>
+    <t>EPM7064AETC44-10N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPLD, 64MCs, 3.3Vcc, 5V tolerant I/Os </t>
+  </si>
+  <si>
+    <t>alternative part for U3; fw can be flashed using JTAG header</t>
+  </si>
+  <si>
+    <t>https://github.com/borti4938/snes_dejitter/tree/regionpatch%2Bdejitter/output_files/multi_func</t>
+  </si>
+  <si>
+    <t>https://github.com/borti4938/snes_dejitter/tree/regionpatch%2Bdejitter/output_files/multi_func_legacy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1336,8 +1356,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1442,7 +1462,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D32" si="0">C7*D$3</f>
+        <f t="shared" ref="D7:D33" si="0">C7*D$3</f>
         <v>3</v>
       </c>
       <c r="E7" t="s">
@@ -1456,8 +1476,8 @@
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" t="s">
-        <v>83</v>
+      <c r="K7" s="14" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1485,39 +1505,35 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" t="s">
-        <v>84</v>
+      <c r="K8" s="14" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
       <c r="B9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>151</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>152</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
+      <c r="K9" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1527,26 +1543,20 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="14" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1556,20 +1566,26 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>78</v>
+        <v>45</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
+      <c r="K11" s="14" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1579,20 +1595,20 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1602,7 +1618,7 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
@@ -1612,10 +1628,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1625,20 +1641,20 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>122</v>
+        <v>50</v>
       </c>
       <c r="G14" t="s">
-        <v>123</v>
+        <v>19</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>53</v>
+        <v>120</v>
+      </c>
+      <c r="B15" t="s">
+        <v>121</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1648,62 +1664,59 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>135</v>
+        <v>52</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>130</v>
+        <v>53</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" t="s">
-        <v>109</v>
+        <v>135</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="C17">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="G17" t="s">
         <v>22</v>
@@ -1713,23 +1726,23 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G18" t="s">
         <v>22</v>
@@ -1739,23 +1752,23 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E19" t="s">
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="G19" t="s">
         <v>22</v>
@@ -1765,10 +1778,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1778,10 +1791,10 @@
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G20" t="s">
         <v>22</v>
@@ -1791,10 +1804,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B21" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1804,59 +1817,59 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G21" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>132</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>133</v>
       </c>
       <c r="G22" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>148</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C23">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G23" t="s">
         <v>22</v>
@@ -1866,23 +1879,23 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>67</v>
+        <v>148</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E24" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>68</v>
+      <c r="F24" t="s">
+        <v>26</v>
       </c>
       <c r="G24" t="s">
         <v>22</v>
@@ -1892,10 +1905,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>66</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -1908,7 +1921,7 @@
         <v>25</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="G25" t="s">
         <v>22</v>
@@ -1918,47 +1931,49 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>134</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E26" t="s">
         <v>25</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="G26" t="s">
         <v>22</v>
       </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>30</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E27" t="s">
         <v>25</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G27" t="s">
         <v>22</v>
@@ -1966,61 +1981,59 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>113</v>
-      </c>
-      <c r="B28" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="C28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>114</v>
-      </c>
-      <c r="F28" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="G28" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28" t="s">
-        <v>115</v>
-      </c>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
+        <v>22</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>136</v>
-      </c>
-      <c r="B29" t="s">
-        <v>140</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B29" s="2"/>
       <c r="C29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>141</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="F29" s="3"/>
       <c r="G29" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="H29" t="s">
+        <v>115</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>137</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>147</v>
+        <v>136</v>
+      </c>
+      <c r="B30" t="s">
+        <v>140</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2033,7 +2046,7 @@
         <v>25</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G30" t="s">
         <v>22</v>
@@ -2043,10 +2056,10 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2059,7 +2072,7 @@
         <v>25</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G31" t="s">
         <v>22</v>
@@ -2069,10 +2082,10 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2085,7 +2098,7 @@
         <v>25</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G32" t="s">
         <v>22</v>
@@ -2094,43 +2107,46 @@
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G33" t="s">
+        <v>22</v>
+      </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>96</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>97</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <f>C35*D$3</f>
-        <v>3</v>
-      </c>
-      <c r="E35" t="s">
-        <v>98</v>
-      </c>
-      <c r="F35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>102</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2140,15 +2156,20 @@
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>103</v>
+        <v>98</v>
+      </c>
+      <c r="F36" t="s">
+        <v>99</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-      <c r="B37" s="3" t="s">
-        <v>104</v>
+      <c r="A37" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>102</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2158,37 +2179,50 @@
         <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="18"/>
-      <c r="B38" s="2" t="s">
-        <v>105</v>
+      <c r="B38" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D38">
         <f>C38*D$3</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>107</v>
-      </c>
-      <c r="F38" s="3"/>
+        <v>106</v>
+      </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <f>C39*D$3</f>
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>107</v>
+      </c>
+      <c r="F39" s="3"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F40" s="3"/>
+      <c r="B40" s="2"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
@@ -2202,39 +2236,44 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F43" s="8"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="10"/>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F43" s="3"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="11"/>
       <c r="F44" s="8"/>
       <c r="H44" s="6"/>
       <c r="I44" s="9"/>
       <c r="J44" s="10"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F45" s="3"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="1"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
+    <row r="45" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="11"/>
+      <c r="F45" s="8"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="10"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F46" s="3"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="1"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A37:A39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2242,8 +2281,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2348,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D21" si="0">C7*D$3</f>
+        <f t="shared" ref="D7:D22" si="0">C7*D$3</f>
         <v>3</v>
       </c>
       <c r="E7" t="s">
@@ -2396,34 +2435,30 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
       <c r="B9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>151</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>152</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
+      <c r="K9" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2433,26 +2468,20 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="14" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2462,20 +2491,26 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>78</v>
+        <v>45</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
+      <c r="K11" s="14" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2485,20 +2520,20 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2508,7 +2543,7 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
@@ -2518,10 +2553,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2531,20 +2566,20 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2554,23 +2589,20 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>108</v>
+        <v>53</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2580,62 +2612,62 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" t="s">
-        <v>109</v>
+        <v>57</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="C17">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="G17" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G18" t="s">
         <v>22</v>
@@ -2645,20 +2677,23 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>31</v>
       </c>
       <c r="G19" t="s">
         <v>22</v>
@@ -2668,23 +2703,20 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C20">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G20" t="s">
         <v>22</v>
@@ -2694,23 +2726,23 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E21" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>68</v>
+      <c r="F21" t="s">
+        <v>26</v>
       </c>
       <c r="G21" t="s">
         <v>22</v>
@@ -2720,23 +2752,23 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22">
-        <f t="shared" ref="D22:D27" si="1">C22*D$3</f>
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
         <v>25</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="G22" t="s">
         <v>22</v>
@@ -2746,23 +2778,23 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D23">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" ref="D23:D28" si="1">C23*D$3</f>
+        <v>9</v>
       </c>
       <c r="E23" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="G23" t="s">
         <v>22</v>
@@ -2772,10 +2804,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -2788,18 +2820,20 @@
         <v>25</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G24" t="s">
         <v>22</v>
       </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2812,7 +2846,7 @@
         <v>25</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G25" t="s">
         <v>22</v>
@@ -2820,23 +2854,23 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E26" t="s">
         <v>25</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G26" t="s">
         <v>22</v>
@@ -2844,67 +2878,68 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>113</v>
-      </c>
-      <c r="B27" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="C27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D27">
         <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28">
         <v>0</v>
       </c>
-      <c r="E27" t="s">
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
         <v>114</v>
       </c>
-      <c r="F27" s="3"/>
-      <c r="G27" t="s">
+      <c r="F28" s="3"/>
+      <c r="G28" t="s">
         <v>13</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H28" t="s">
         <v>115</v>
       </c>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>96</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>97</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <f>C30*D$3</f>
-        <v>3</v>
-      </c>
-      <c r="E30" t="s">
-        <v>98</v>
-      </c>
-      <c r="F30" t="s">
-        <v>99</v>
-      </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>102</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2914,15 +2949,20 @@
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>103</v>
+        <v>98</v>
+      </c>
+      <c r="F31" t="s">
+        <v>99</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="3" t="s">
-        <v>104</v>
+      <c r="A32" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>102</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2932,37 +2972,50 @@
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
-      <c r="B33" s="2" t="s">
-        <v>105</v>
+      <c r="B33" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <f>C33*D$3</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>107</v>
-      </c>
-      <c r="F33" s="3"/>
+        <v>106</v>
+      </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <f>C34*D$3</f>
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" s="3"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F35" s="3"/>
+      <c r="B35" s="2"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
@@ -2976,39 +3029,44 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F38" s="8"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="10"/>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F38" s="3"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="11"/>
       <c r="F39" s="8"/>
       <c r="H39" s="6"/>
       <c r="I39" s="9"/>
       <c r="J39" s="10"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F40" s="3"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="1"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
+    <row r="40" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="11"/>
+      <c r="F40" s="8"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="10"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F41" s="3"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="1"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A32:A34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3016,7 +3074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3168,8 +3226,8 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" t="s">
-        <v>84</v>
+      <c r="K8" s="14" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>